<commit_message>
Adding Song list excel sheet and problem 3 solution
</commit_message>
<xml_diff>
--- a/MATH425_Fall2025_roster - Copy.xlsx
+++ b/MATH425_Fall2025_roster - Copy.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29415"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10916"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\working\waccache\BY3PEPF0001804B\EXCELCNV\282e71c2-0fef-410c-af99-e27095a30c18\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tybo/Documents/AppldLinAlgb-Project1/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{CE1C4B66-B880-44DB-975C-BE61FE3558C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486A071D-EDB8-A047-AB2B-CFF63EF8104C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="15480" windowHeight="11640" xr2:uid="{B60E26F7-25E1-40BB-8CF6-AD931B1BA544}"/>
+    <workbookView xWindow="0" yWindow="860" windowWidth="34200" windowHeight="21380" xr2:uid="{B60E26F7-25E1-40BB-8CF6-AD931B1BA544}"/>
   </bookViews>
   <sheets>
     <sheet name="in" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
   <si>
     <t>Aviles,Francis Jake</t>
   </si>
@@ -129,13 +129,16 @@
   </si>
   <si>
     <t>Zhu,Breanna</t>
+  </si>
+  <si>
+    <t>Henry, Boateng</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="19">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -459,7 +462,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -589,6 +592,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -634,9 +648,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -698,9 +715,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -738,7 +755,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -844,7 +861,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -986,7 +1003,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -994,170 +1011,175 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{36AB49F9-A29F-4E42-A082-21ACB55BF96C}">
-  <dimension ref="A1:A31"/>
+  <dimension ref="A1:A32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:1">
+    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1">
+    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="11" spans="1:1">
+    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="12" spans="1:1">
+    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:1">
+    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A13" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:1">
+    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A14" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="15" spans="1:1">
+    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A15" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:1">
+    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A16" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="17" spans="1:1">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="1:1">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:1">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="21" spans="1:1">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:1">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="23" spans="1:1">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="24" spans="1:1">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="25" spans="1:1">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A25" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="26" spans="1:1">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="27" spans="1:1">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:1">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:1">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="30" spans="1:1">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="31" spans="1:1">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A32" s="2" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>